<commit_message>
Creating suggestions for correcting quality failures.
</commit_message>
<xml_diff>
--- a/schema/Copaf_aix/issues_metadados_copaf_aix.xlsx
+++ b/schema/Copaf_aix/issues_metadados_copaf_aix.xlsx
@@ -19546,7 +19546,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Total number of cells in schema</t>
+          <t>Total number of cells in schema (sum of columns x rows for each table)</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -19744,7 +19744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19793,6 +19793,26 @@
           <t>limit</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>SUGGESTED_VALUE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SUGGESTED_SOURCE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SUGGESTED_CONFIDENCE</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SUGGESTED_DDL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -19823,6 +19843,24 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Codigo de tip tra itcd.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>RULES</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>COMMENT ON COLUMN COPAF_AIX.DEBITO.COD_TIP_TRA_ITCD IS 'Codigo de tip tra itcd.';</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>